<commit_message>
Updated Excel sheet -- only one data point is missing
</commit_message>
<xml_diff>
--- a/tensorflow_MNIST/MNIST master-worker results.xlsx
+++ b/tensorflow_MNIST/MNIST master-worker results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="batch size = 20" sheetId="4" r:id="rId1"/>
@@ -468,6 +468,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.90139999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.91600000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1182,6 +1185,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.91900000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.91720000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3981,8 +3987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4164,6 +4170,9 @@
       <c r="B16">
         <v>0.90949999999999998</v>
       </c>
+      <c r="C16">
+        <v>0.91600000000000004</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -4183,8 +4192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4400,6 +4409,9 @@
       </c>
       <c r="C15">
         <v>0.92510000000000003</v>
+      </c>
+      <c r="D15">
+        <v>0.91720000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>